<commit_message>
Updated CLR/OLR metadata based on test ingest QA
</commit_message>
<xml_diff>
--- a/course_catalogs/CLR/CLR_standard_input_course_catalogs.xlsx
+++ b/course_catalogs/CLR/CLR_standard_input_course_catalogs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\UCSD-course-catalogs\CLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\course_catalogs\CLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2086,13 +2086,14 @@
     <t>Past catalogs @ http://blink.ucsd.edu/instructors/resources/catalog.html</t>
   </si>
   <si>
-    <t>Selected volumes of UC San Diego’s General Catalog or Course Catalog have been digitized and are full-text searchable in this collection. They list the degree requirements and descriptions for colleges, departments, and schools offered by the University of California, San Diego, with course descriptions for each course.  Student/faculty profiles and photographs also offer a glimpse of campus life. The Official Catalog of Record is an archival document of record and does not reflect interim updates that may take place during the period between official publications. UC San Diego may publish interim updates to the catalog for information and advising purposes only.</t>
-  </si>
-  <si>
     <t>University of California, San Diego</t>
   </si>
   <si>
     <t>UC San Diego General Catalog test</t>
+  </si>
+  <si>
+    <t>Selected volumes of UC San Diego’s General Catalog or Course Catalog have been digitized and are full-text searchable in this collection. They list the degree requirements and descriptions for colleges, departments, and schools offered by the University of California, San Diego, with course descriptions for each course.  Student/faculty profiles and photographs also offer a glimpse of campus life. The Official Catalog of Record is an archival document of record and does not reflect interim updates that may take place during the period between official publications. UC San Diego may publish interim updates to the catalog for information and advising purposes only.
+If you would like a higher quality version of the catalog, please contact Special Collections &amp; Archives.</t>
   </si>
 </sst>
 </file>
@@ -3140,8 +3141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,7 +3209,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>357</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>636</v>
@@ -3240,13 +3241,13 @@
         <v>635</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>637</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>638</v>

</xml_diff>

<commit_message>
Updated OLR with input from QA
</commit_message>
<xml_diff>
--- a/course_catalogs/CLR/CLR_standard_input_course_catalogs.xlsx
+++ b/course_catalogs/CLR/CLR_standard_input_course_catalogs.xlsx
@@ -2089,11 +2089,11 @@
     <t>University of California, San Diego</t>
   </si>
   <si>
-    <t>UC San Diego General Catalog test</t>
-  </si>
-  <si>
     <t>Selected volumes of UC San Diego’s General Catalog or Course Catalog have been digitized and are full-text searchable in this collection. They list the degree requirements and descriptions for colleges, departments, and schools offered by the University of California, San Diego, with course descriptions for each course.  Student/faculty profiles and photographs also offer a glimpse of campus life. The Official Catalog of Record is an archival document of record and does not reflect interim updates that may take place during the period between official publications. UC San Diego may publish interim updates to the catalog for information and advising purposes only.
 If you would like a higher quality version of the catalog, please contact Special Collections &amp; Archives.</t>
+  </si>
+  <si>
+    <t>UC San Diego General Catalog</t>
   </si>
 </sst>
 </file>
@@ -3141,8 +3141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3209,7 +3209,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="330" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>357</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>636</v>
@@ -3241,7 +3241,7 @@
         <v>635</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>637</v>

</xml_diff>